<commit_message>
Update tests to include microcells
</commit_message>
<xml_diff>
--- a/tests/path_loss_validation_etsi_3gpp_tr_138_901.xlsx
+++ b/tests/path_loss_validation_etsi_3gpp_tr_138_901.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\pysim5g\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA6DB27-9AFD-4AF6-A11D-28343030AF69}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF793A1-23DD-4BDA-91EB-91B94BFC2EA5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="14415" windowHeight="13290" xr2:uid="{EF8BEF9E-9108-4BFF-B78C-39BCF7F44F4E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{EF8BEF9E-9108-4BFF-B78C-39BCF7F44F4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="48">
   <si>
     <t>LOS</t>
   </si>
@@ -141,9 +141,6 @@
     <t>d_apost_bp</t>
   </si>
   <si>
-    <t>uMA NLOS Optional model</t>
-  </si>
-  <si>
     <t>Frequency (GHz)</t>
   </si>
   <si>
@@ -157,12 +154,36 @@
   </si>
   <si>
     <t>Receiver height</t>
+  </si>
+  <si>
+    <t>Umi LOS</t>
+  </si>
+  <si>
+    <t>Umi NLOS</t>
+  </si>
+  <si>
+    <t>UMa NLOS Optional model</t>
+  </si>
+  <si>
+    <t>pl_apost_umi_nlos</t>
+  </si>
+  <si>
+    <t>pl_umi_nlos</t>
+  </si>
+  <si>
+    <t>pl_apost_uma_nlos</t>
+  </si>
+  <si>
+    <t>pl_uma_nlos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -359,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -440,6 +461,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -461,38 +515,11 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -808,18 +835,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3F976F-A889-4452-9B55-F1E5AA192C6F}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -927,15 +954,15 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="32"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="43"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
@@ -1031,15 +1058,15 @@
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="32"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="43"/>
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1095,15 +1122,15 @@
       <c r="A21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="33">
+      <c r="B21" s="44">
         <f>IF(AND(SUM(C20:D20)&gt;=10,SUM(C20:D20)&lt;=5000),MAX(B14,B20))</f>
         <v>79.009197673455859</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="34"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="45"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
@@ -1135,15 +1162,15 @@
       <c r="A23" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B23" s="39">
         <f>IF(AND(SUM(C22:D22)&gt;=10,SUM(C22:D22)&lt;=5000),MAX(B22,B22))</f>
         <v>143.75425407467171</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="29"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
@@ -1156,15 +1183,15 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="43"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
@@ -1260,15 +1287,15 @@
       <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="32"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="43"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
@@ -1295,7 +1322,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B34" s="3">
         <f>13.54+39.08*LOG10(E34)+20*LOG10(F34)-0.6*($C$5-1.5)</f>
@@ -1321,21 +1348,21 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="33">
+        <v>47</v>
+      </c>
+      <c r="B35" s="44">
         <f>IF(AND(SUM(C34:D34)&gt;=10,SUM(C34:D34)&lt;=5000),MAX(B28,B34))</f>
         <v>89.50456523385148</v>
       </c>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="34"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="45"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B36" s="3">
         <f>13.54+39.08*LOG10(E36)+20*LOG10(F36)-0.6*($C$5-1.5)</f>
@@ -1361,57 +1388,57 @@
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="28">
+        <v>47</v>
+      </c>
+      <c r="B37" s="39">
         <f>IF(AND(SUM(C36:D36)&gt;=10,SUM(C36:D36)&lt;=5000),MAX(B36,B36))</f>
         <v>154.99808950285214</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="29"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="40"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="38"/>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="37"/>
-    </row>
-    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
+      <c r="B40" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="45" t="s">
+      <c r="C40" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="D40" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="45" t="s">
+      <c r="E40" s="35" t="s">
         <v>40</v>
-      </c>
-      <c r="E40" s="45" t="s">
-        <v>41</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="38">
+      <c r="A41" s="28">
         <v>3.5</v>
       </c>
       <c r="B41" s="1">
         <v>500</v>
       </c>
-      <c r="C41" s="39">
+      <c r="C41" s="29">
         <f>SQRT(POWER(B41,2)+POWER((D41-E41),2))</f>
         <v>501.12099337385575</v>
       </c>
@@ -1421,19 +1448,19 @@
       <c r="E41" s="1">
         <v>1.5</v>
       </c>
-      <c r="F41" s="40">
+      <c r="F41" s="30">
         <f>32.4+20*LOG10(A41)+30*LOG10(C41)</f>
         <v>124.27963879538905</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="38">
+      <c r="A42" s="28">
         <v>3.5</v>
       </c>
       <c r="B42" s="1">
         <v>1000</v>
       </c>
-      <c r="C42" s="39">
+      <c r="C42" s="29">
         <f>SQRT(POWER(B42,2)+POWER((D42-E42),2))</f>
         <v>1000.4060425647178</v>
       </c>
@@ -1443,19 +1470,19 @@
       <c r="E42" s="1">
         <v>1.5</v>
       </c>
-      <c r="F42" s="40">
+      <c r="F42" s="30">
         <f>32.4+20*LOG10(A42)+30*LOG10(C42)</f>
         <v>133.28665007461876</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="38">
+      <c r="A43" s="28">
         <v>3.5</v>
       </c>
       <c r="B43" s="1">
         <v>5000</v>
       </c>
-      <c r="C43" s="39">
+      <c r="C43" s="29">
         <f>SQRT(POWER(B43,2)+POWER((D43-E43),2))</f>
         <v>5000.0812243402606</v>
       </c>
@@ -1465,19 +1492,19 @@
       <c r="E43" s="1">
         <v>1.5</v>
       </c>
-      <c r="F43" s="40">
+      <c r="F43" s="30">
         <f>32.4+20*LOG10(A43)+30*LOG10(C43)</f>
         <v>154.25067266706358</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="38">
+      <c r="A44" s="28">
         <v>3.5</v>
       </c>
       <c r="B44" s="1">
         <v>10000</v>
       </c>
-      <c r="C44" s="39">
+      <c r="C44" s="29">
         <f>SQRT(POWER(B44,2)+POWER((D44-E44),2))</f>
         <v>10000.040612417532</v>
       </c>
@@ -1487,19 +1514,19 @@
       <c r="E44" s="1">
         <v>1.5</v>
       </c>
-      <c r="F44" s="40">
+      <c r="F44" s="30">
         <f>32.4+20*LOG10(A44)+30*LOG10(C44)</f>
         <v>163.28141380014455</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="41">
+      <c r="A45" s="31">
         <v>3.5</v>
       </c>
       <c r="B45" s="20">
         <v>20000</v>
       </c>
-      <c r="C45" s="42">
+      <c r="C45" s="32">
         <f>SQRT(POWER(B45,2)+POWER((D45-E45),2))</f>
         <v>20000.02030623969</v>
       </c>
@@ -1509,13 +1536,338 @@
       <c r="E45" s="20">
         <v>1.5</v>
       </c>
-      <c r="F45" s="43">
+      <c r="F45" s="33">
         <f>32.4+20*LOG10(A45)+30*LOG10(C45)</f>
         <v>172.31227398525002</v>
       </c>
     </row>
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="26">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="26">
+        <f>C50-C51</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="26">
+        <f>C51-C49</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" s="42"/>
+      <c r="C58" s="42"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="42"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="43"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="46">
+        <f>32.4+21*LOG10(E60)+20*LOG10(F60)</f>
+        <v>86.249057334586922</v>
+      </c>
+      <c r="C60" s="3">
+        <v>90</v>
+      </c>
+      <c r="D60" s="3">
+        <v>10</v>
+      </c>
+      <c r="E60" s="7">
+        <f>SQRT(POWER((C60+D60),2)+POWER(($C$4-$C$5),2))</f>
+        <v>105.46207849269803</v>
+      </c>
+      <c r="F60" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="G60" s="12">
+        <f>4*$C$52*$C$53*(F60*1000000000)/300000000</f>
+        <v>209.66666666666666</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="47">
+        <f>32.4+40*LOG10(E61)+20*LOG10($F$61)-9.5*LOG10(POWER(G61,2)+POWER($C$50-$C$51,2))</f>
+        <v>147.60739080356535</v>
+      </c>
+      <c r="C61" s="18">
+        <v>4990</v>
+      </c>
+      <c r="D61" s="18">
+        <v>10</v>
+      </c>
+      <c r="E61" s="19">
+        <f>SQRT(POWER((C61+D61),2)+POWER(($C$4-$C$5),2))</f>
+        <v>5000.1122237405834</v>
+      </c>
+      <c r="F61" s="20">
+        <v>3.7</v>
+      </c>
+      <c r="G61" s="21">
+        <f>4*$C$52*$C$53*(F61*1000000000)/300000000</f>
+        <v>209.66666666666666</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="8"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="4"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="8"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" s="42"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="43"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="3">
+        <f>35.3*LOG10(E66)+22.4+21.3*LOG10(F66)-0.3*($C$51-1.5)</f>
+        <v>105.91799704260886</v>
+      </c>
+      <c r="C66" s="3">
+        <v>90</v>
+      </c>
+      <c r="D66" s="3">
+        <v>10</v>
+      </c>
+      <c r="E66" s="7">
+        <f>SQRT(POWER((C66+D66),2)+POWER(($C$4-$C$5),2))</f>
+        <v>105.46207849269803</v>
+      </c>
+      <c r="F66" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="G66" s="12">
+        <f>4*$C$52*$C$53*(F66*1000000000)/300000000</f>
+        <v>209.66666666666666</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B67" s="44">
+        <f>IF(AND(SUM(C66:D66)&gt;=10,SUM(C66:D66)&lt;=5000),MAX(B60,B66))</f>
+        <v>105.91799704260886</v>
+      </c>
+      <c r="C67" s="44"/>
+      <c r="D67" s="44"/>
+      <c r="E67" s="44"/>
+      <c r="F67" s="44"/>
+      <c r="G67" s="45"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68" s="3">
+        <f>35.3*LOG10(E68)+22.4+21.3*LOG10(F68)-0.3*($C$51-1.5)</f>
+        <v>165.07668196317499</v>
+      </c>
+      <c r="C68" s="3">
+        <v>4990</v>
+      </c>
+      <c r="D68" s="3">
+        <v>10</v>
+      </c>
+      <c r="E68" s="7">
+        <f>SQRT(POWER((C68+D68),2)+POWER(($C$4-$C$5),2))</f>
+        <v>5000.1122237405834</v>
+      </c>
+      <c r="F68" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="G68" s="12">
+        <f>4*$C$52*$C$53*(F68*1000000000)/300000000</f>
+        <v>209.66666666666666</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B69" s="39">
+        <f>IF(AND(SUM(C68:D68)&gt;=10,SUM(C68:D68)&lt;=5000),MAX(B68,B68))</f>
+        <v>165.07668196317499</v>
+      </c>
+      <c r="C69" s="39"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
+      <c r="G69" s="40"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A64:G64"/>
+    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="B69:G69"/>
     <mergeCell ref="A39:F39"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="A12:G12"/>
@@ -1527,7 +1879,7 @@
     <mergeCell ref="B23:G23"/>
   </mergeCells>
   <conditionalFormatting sqref="F42:F43">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1541,7 +1893,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1555,7 +1907,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1569,7 +1921,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>